<commit_message>
modified:   main.py 	modified:   novos_users_ac.py 	modified:   repl/analise_semanas.ipynb
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -2401,7 +2401,7 @@
         </is>
       </c>
       <c r="NE2" s="2" t="n">
-        <v>45688.60844012025</v>
+        <v>45688.8319918787</v>
       </c>
       <c r="NF2" s="2" t="inlineStr"/>
       <c r="NG2" s="2" t="inlineStr"/>
@@ -19037,6 +19037,21 @@
       <c r="NG20" s="18" t="n">
         <v>-0.1457579561397032</v>
       </c>
+      <c r="NI20" s="16" t="n">
+        <v>4073</v>
+      </c>
+      <c r="NJ20" s="16" t="n">
+        <v>7526</v>
+      </c>
+      <c r="NK20" s="16" t="n">
+        <v>6925</v>
+      </c>
+      <c r="NL20" s="16" t="n">
+        <v>6563</v>
+      </c>
+      <c r="NM20" s="16" t="n">
+        <v>9620</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="15" t="inlineStr">
@@ -20151,6 +20166,21 @@
       <c r="NG21" s="18" t="n">
         <v>0.2486817127188357</v>
       </c>
+      <c r="NI21" s="16" t="n">
+        <v>1825</v>
+      </c>
+      <c r="NJ21" s="16" t="n">
+        <v>2398</v>
+      </c>
+      <c r="NK21" s="16" t="n">
+        <v>-841</v>
+      </c>
+      <c r="NL21" s="16" t="n">
+        <v>486</v>
+      </c>
+      <c r="NM21" s="16" t="n">
+        <v>2052</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="15" t="inlineStr">
@@ -21265,6 +21295,21 @@
       <c r="NG22" s="18" t="n">
         <v>0.3305166122527368</v>
       </c>
+      <c r="NI22" s="16" t="n">
+        <v>1599</v>
+      </c>
+      <c r="NJ22" s="16" t="n">
+        <v>2946</v>
+      </c>
+      <c r="NK22" s="16" t="n">
+        <v>-637</v>
+      </c>
+      <c r="NL22" s="16" t="n">
+        <v>838</v>
+      </c>
+      <c r="NM22" s="16" t="n">
+        <v>2182</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" s="15" t="inlineStr">
@@ -22379,6 +22424,21 @@
       <c r="NG23" s="18" t="n">
         <v>0.278217109992811</v>
       </c>
+      <c r="NI23" s="16" t="n">
+        <v>-261</v>
+      </c>
+      <c r="NJ23" s="16" t="n">
+        <v>-959</v>
+      </c>
+      <c r="NK23" s="16" t="n">
+        <v>-868</v>
+      </c>
+      <c r="NL23" s="16" t="n">
+        <v>-869</v>
+      </c>
+      <c r="NM23" s="16" t="n">
+        <v>-599</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" s="15" t="inlineStr">
@@ -23493,6 +23553,21 @@
       <c r="NG24" s="18" t="n">
         <v>0.1012956419316844</v>
       </c>
+      <c r="NI24" s="16" t="n">
+        <v>354</v>
+      </c>
+      <c r="NJ24" s="16" t="n">
+        <v>262</v>
+      </c>
+      <c r="NK24" s="16" t="n">
+        <v>537</v>
+      </c>
+      <c r="NL24" s="16" t="n">
+        <v>375</v>
+      </c>
+      <c r="NM24" s="16" t="n">
+        <v>342</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="15" t="inlineStr">
@@ -24607,6 +24682,21 @@
       <c r="NG25" s="18" t="n">
         <v>0.09708737864077666</v>
       </c>
+      <c r="NI25" s="16" t="n">
+        <v>133</v>
+      </c>
+      <c r="NJ25" s="16" t="n">
+        <v>149</v>
+      </c>
+      <c r="NK25" s="16" t="n">
+        <v>127</v>
+      </c>
+      <c r="NL25" s="16" t="n">
+        <v>142</v>
+      </c>
+      <c r="NM25" s="16" t="n">
+        <v>127</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="15" t="inlineStr">
@@ -25721,6 +25811,21 @@
       <c r="NG26" s="18" t="n">
         <v>0.9268292682926829</v>
       </c>
+      <c r="NI26" s="16" t="n">
+        <v>31</v>
+      </c>
+      <c r="NJ26" s="16" t="n">
+        <v>38</v>
+      </c>
+      <c r="NK26" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="NL26" s="16" t="n">
+        <v>33</v>
+      </c>
+      <c r="NM26" s="16" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" s="15" t="inlineStr">
@@ -26835,6 +26940,21 @@
       <c r="NG27" s="18" t="n">
         <v>0.7432098765432098</v>
       </c>
+      <c r="NI27" s="16" t="n">
+        <v>79</v>
+      </c>
+      <c r="NJ27" s="16" t="n">
+        <v>112</v>
+      </c>
+      <c r="NK27" s="16" t="n">
+        <v>157</v>
+      </c>
+      <c r="NL27" s="16" t="n">
+        <v>165</v>
+      </c>
+      <c r="NM27" s="16" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="15" t="inlineStr">
@@ -27949,6 +28069,21 @@
       <c r="NG28" s="18" t="n">
         <v>0.6914285714285715</v>
       </c>
+      <c r="NI28" s="16" t="n">
+        <v>55</v>
+      </c>
+      <c r="NJ28" s="16" t="n">
+        <v>106</v>
+      </c>
+      <c r="NK28" s="16" t="n">
+        <v>130</v>
+      </c>
+      <c r="NL28" s="16" t="n">
+        <v>139</v>
+      </c>
+      <c r="NM28" s="16" t="n">
+        <v>162</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="15" t="inlineStr">
@@ -29063,6 +29198,21 @@
       <c r="NG29" s="18" t="n">
         <v>1.072727272727273</v>
       </c>
+      <c r="NI29" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="NJ29" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="NK29" s="16" t="n">
+        <v>27</v>
+      </c>
+      <c r="NL29" s="16" t="n">
+        <v>26</v>
+      </c>
+      <c r="NM29" s="16" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" s="19" t="inlineStr">
@@ -30176,6 +30326,21 @@
       </c>
       <c r="NG30" s="10" t="n">
         <v>0.09803921568627461</v>
+      </c>
+      <c r="NI30" s="16" t="n">
+        <v>156</v>
+      </c>
+      <c r="NJ30" s="16" t="n">
+        <v>157</v>
+      </c>
+      <c r="NK30" s="16" t="n">
+        <v>151</v>
+      </c>
+      <c r="NL30" s="16" t="n">
+        <v>168</v>
+      </c>
+      <c r="NM30" s="16" t="n">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   logins.py 	modified:   logins_tv.py 	modified:   main.py 	modified:   novos_users_ac.py
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -122,10 +122,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="4" fillId="3" borderId="2"/>
     <xf numFmtId="169" fontId="3" fillId="3" borderId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="3" borderId="2"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="3"/>
     <xf numFmtId="166" fontId="3" fillId="3" borderId="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -148,7 +148,7 @@
     </xf>
     <xf numFmtId="169" fontId="4" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="12"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="8"/>
-    <xf numFmtId="169" fontId="4" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="19"/>
+    <xf numFmtId="169" fontId="4" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="18"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="5"/>
     <xf numFmtId="166" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="10">
       <alignment horizontal="right" vertical="center"/>
@@ -159,7 +159,7 @@
     <xf numFmtId="169" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="16">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="18">
+    <xf numFmtId="169" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="19">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -198,8 +198,8 @@
     <cellStyle name="totalinhadir" xfId="15" hidden="0"/>
     <cellStyle name="normalgrayunderperc" xfId="16" hidden="0"/>
     <cellStyle name="monthyearsimple" xfId="17" hidden="0"/>
-    <cellStyle name="normalgrayunderpercenter" xfId="18" hidden="0"/>
-    <cellStyle name="tlinhagraypercenter" xfId="19" hidden="0"/>
+    <cellStyle name="tlinhagraypercenter" xfId="18" hidden="0"/>
+    <cellStyle name="normalgrayunderpercenter" xfId="19" hidden="0"/>
     <cellStyle name="nmgrdsund" xfId="20" hidden="0"/>
     <cellStyle name="normalalgray" xfId="21" hidden="0"/>
     <cellStyle name="nmgrdseuro" xfId="22" hidden="0"/>
@@ -2424,7 +2424,7 @@
         </is>
       </c>
       <c r="NE2" s="2" t="n">
-        <v>45688.49436583371</v>
+        <v>45688.51418173204</v>
       </c>
       <c r="NF2" s="2" t="inlineStr"/>
       <c r="NG2" s="2" t="inlineStr"/>
@@ -2478,7 +2478,7 @@
         </is>
       </c>
       <c r="OE2" s="4" t="inlineStr"/>
-      <c r="OF2" s="4" t="inlineStr"/>
+      <c r="OF2" s="6" t="inlineStr"/>
       <c r="OH2" s="6" t="inlineStr">
         <is>
           <t>AsIs</t>
@@ -3701,12 +3701,12 @@
       </c>
       <c r="OF3" s="11" t="inlineStr">
         <is>
-          <t>31/Jan</t>
+          <t>Avg.YTD</t>
         </is>
       </c>
       <c r="OH3" s="11" t="inlineStr">
         <is>
-          <t>Avg.4m</t>
+          <t>25/Jan</t>
         </is>
       </c>
     </row>
@@ -4899,9 +4899,7 @@
       <c r="OE6" s="4" t="n">
         <v>0.05370001020683013</v>
       </c>
-      <c r="OF6" s="4" t="n">
-        <v>-1</v>
-      </c>
+      <c r="OF6" s="4" t="inlineStr"/>
       <c r="OH6" s="4" t="inlineStr"/>
     </row>
     <row r="7">
@@ -6083,9 +6081,7 @@
       <c r="OE7" s="18" t="n">
         <v>0.05993024468459773</v>
       </c>
-      <c r="OF7" s="18" t="n">
-        <v>0</v>
-      </c>
+      <c r="OF7" s="18" t="inlineStr"/>
       <c r="OH7" s="18" t="inlineStr"/>
     </row>
     <row r="8">
@@ -7267,9 +7263,7 @@
       <c r="OE8" s="18" t="n">
         <v>-0.08308284466209037</v>
       </c>
-      <c r="OF8" s="18" t="n">
-        <v>0</v>
-      </c>
+      <c r="OF8" s="18" t="inlineStr"/>
       <c r="OH8" s="18" t="inlineStr"/>
     </row>
     <row r="9">
@@ -8451,9 +8445,7 @@
       <c r="OE9" s="18" t="n">
         <v>-0.08021612635078967</v>
       </c>
-      <c r="OF9" s="18" t="n">
-        <v>0</v>
-      </c>
+      <c r="OF9" s="18" t="inlineStr"/>
       <c r="OH9" s="18" t="inlineStr"/>
     </row>
     <row r="10">
@@ -9633,9 +9625,7 @@
       <c r="OE10" s="18" t="n">
         <v>-1</v>
       </c>
-      <c r="OF10" s="18" t="n">
-        <v>0</v>
-      </c>
+      <c r="OF10" s="18" t="inlineStr"/>
       <c r="OH10" s="18" t="inlineStr"/>
     </row>
     <row r="11">
@@ -10817,9 +10807,7 @@
       <c r="OE11" s="18" t="n">
         <v>0.1334055898902315</v>
       </c>
-      <c r="OF11" s="18" t="n">
-        <v>0</v>
-      </c>
+      <c r="OF11" s="18" t="inlineStr"/>
       <c r="OH11" s="18" t="inlineStr"/>
     </row>
     <row r="12">
@@ -12001,9 +11989,7 @@
       <c r="OE12" s="18" t="n">
         <v>0.02296896255833913</v>
       </c>
-      <c r="OF12" s="18" t="n">
-        <v>0</v>
-      </c>
+      <c r="OF12" s="18" t="inlineStr"/>
       <c r="OH12" s="18" t="inlineStr"/>
     </row>
     <row r="13">
@@ -13206,7 +13192,7 @@
       <c r="OC14" s="5" t="inlineStr"/>
       <c r="OD14" s="18" t="inlineStr"/>
       <c r="OE14" s="18" t="inlineStr"/>
-      <c r="OF14" s="18" t="inlineStr"/>
+      <c r="OF14" s="17" t="inlineStr"/>
       <c r="OH14" s="17" t="inlineStr"/>
     </row>
     <row r="15">
@@ -14388,9 +14374,7 @@
       <c r="OE15" s="18" t="n">
         <v>-0.04980534731829733</v>
       </c>
-      <c r="OF15" s="18" t="n">
-        <v>-0.03820448336378923</v>
-      </c>
+      <c r="OF15" s="17" t="inlineStr"/>
       <c r="OH15" s="17" t="inlineStr"/>
     </row>
     <row r="16">
@@ -15572,9 +15556,7 @@
       <c r="OE16" s="18" t="n">
         <v>-0.05138017111355542</v>
       </c>
-      <c r="OF16" s="18" t="n">
-        <v>-0.03159371599610483</v>
-      </c>
+      <c r="OF16" s="17" t="inlineStr"/>
       <c r="OH16" s="17" t="inlineStr"/>
     </row>
     <row r="17">
@@ -16756,9 +16738,7 @@
       <c r="OE17" s="18" t="n">
         <v>-0.07079431577700357</v>
       </c>
-      <c r="OF17" s="18" t="n">
-        <v>-0.04529535759929626</v>
-      </c>
+      <c r="OF17" s="17" t="inlineStr"/>
       <c r="OH17" s="17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -17933,7 +17913,7 @@
         <v>0.02243596094822098</v>
       </c>
       <c r="OF18" s="10" t="inlineStr"/>
-      <c r="OH18" s="17" t="inlineStr"/>
+      <c r="OH18" s="10" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="B19" s="13" t="inlineStr">
@@ -19084,7 +19064,7 @@
         <v>0.4657930824318146</v>
       </c>
       <c r="NO20" s="18" t="n">
-        <v>0.5338621596842987</v>
+        <v>0.5888352120236178</v>
       </c>
       <c r="NP20" s="18" t="n">
         <v>0.5338621596842987</v>
@@ -19131,9 +19111,7 @@
       <c r="OE20" s="18" t="n">
         <v>-0.09620717940705437</v>
       </c>
-      <c r="OF20" s="18" t="n">
-        <v>0.07456366495655986</v>
-      </c>
+      <c r="OF20" s="18" t="inlineStr"/>
       <c r="OH20" s="17" t="n">
         <v>35584</v>
       </c>
@@ -20317,9 +20295,7 @@
       <c r="OE21" s="18" t="n">
         <v>-0.1190148443022434</v>
       </c>
-      <c r="OF21" s="18" t="n">
-        <v>0.07753359352489719</v>
-      </c>
+      <c r="OF21" s="18" t="inlineStr"/>
       <c r="OH21" s="17" t="n">
         <v>1532705</v>
       </c>
@@ -21503,9 +21479,7 @@
       <c r="OE22" s="18" t="n">
         <v>0.08640426532852441</v>
       </c>
-      <c r="OF22" s="18" t="n">
-        <v>0.1109136608872452</v>
-      </c>
+      <c r="OF22" s="18" t="inlineStr"/>
       <c r="OH22" s="17" t="n">
         <v>1271715</v>
       </c>
@@ -22689,9 +22663,7 @@
       <c r="OE23" s="18" t="n">
         <v>0.7711368447266842</v>
       </c>
-      <c r="OF23" s="18" t="n">
-        <v>0.6649214659685864</v>
-      </c>
+      <c r="OF23" s="18" t="inlineStr"/>
       <c r="OH23" s="17" t="n">
         <v>157669</v>
       </c>
@@ -23875,9 +23847,7 @@
       <c r="OE24" s="18" t="n">
         <v>0.1207671561282588</v>
       </c>
-      <c r="OF24" s="18" t="n">
-        <v>0.1537196876284423</v>
-      </c>
+      <c r="OF24" s="18" t="inlineStr"/>
       <c r="OH24" s="17" t="n">
         <v>51448</v>
       </c>
@@ -25061,9 +25031,7 @@
       <c r="OE25" s="18" t="n">
         <v>-0.005865102639296182</v>
       </c>
-      <c r="OF25" s="18" t="n">
-        <v>0.09584393553859202</v>
-      </c>
+      <c r="OF25" s="18" t="inlineStr"/>
       <c r="OH25" s="17" t="n">
         <v>51873</v>
       </c>
@@ -26247,9 +26215,7 @@
       <c r="OE26" s="18" t="n">
         <v>-0.06231454005934722</v>
       </c>
-      <c r="OF26" s="18" t="n">
-        <v>0.1268057784911718</v>
-      </c>
+      <c r="OF26" s="18" t="inlineStr"/>
       <c r="OH26" s="17" t="n">
         <v>19691</v>
       </c>
@@ -27433,9 +27399,7 @@
       <c r="OE27" s="18" t="n">
         <v>0.124203821656051</v>
       </c>
-      <c r="OF27" s="18" t="n">
-        <v>0.118875231520458</v>
-      </c>
+      <c r="OF27" s="18" t="inlineStr"/>
       <c r="OH27" s="17" t="n">
         <v>122590</v>
       </c>
@@ -28619,9 +28583,7 @@
       <c r="OE28" s="18" t="n">
         <v>0.1734390485629336</v>
       </c>
-      <c r="OF28" s="18" t="n">
-        <v>0.1122062168309325</v>
-      </c>
+      <c r="OF28" s="18" t="inlineStr"/>
       <c r="OH28" s="17" t="n">
         <v>106022</v>
       </c>
@@ -29805,9 +29767,7 @@
       <c r="OE29" s="18" t="n">
         <v>-0.07692307692307687</v>
       </c>
-      <c r="OF29" s="18" t="n">
-        <v>0.1719457013574661</v>
-      </c>
+      <c r="OF29" s="18" t="inlineStr"/>
       <c r="OH29" s="17" t="n">
         <v>16568</v>
       </c>
@@ -30991,10 +30951,8 @@
       <c r="OE30" s="10" t="n">
         <v>-0.02457231726283049</v>
       </c>
-      <c r="OF30" s="10" t="n">
-        <v>0.1005257084241569</v>
-      </c>
-      <c r="OH30" s="17" t="n">
+      <c r="OF30" s="10" t="inlineStr"/>
+      <c r="OH30" s="8" t="n">
         <v>63880</v>
       </c>
     </row>
@@ -32150,7 +32108,7 @@
         <v>0.06020066889632103</v>
       </c>
       <c r="NP32" s="18" t="n">
-        <v>0.06020066889632103</v>
+        <v>0.034257748776509</v>
       </c>
       <c r="NR32" s="16" t="n">
         <v>1543</v>
@@ -32194,9 +32152,7 @@
       <c r="OE32" s="18" t="n">
         <v>-0.03275348691427671</v>
       </c>
-      <c r="OF32" s="18" t="n">
-        <v>0.04177609313659131</v>
-      </c>
+      <c r="OF32" s="18" t="inlineStr"/>
       <c r="OH32" s="18" t="inlineStr"/>
     </row>
     <row r="33">
@@ -33334,7 +33290,7 @@
         <v>0.6155339805825242</v>
       </c>
       <c r="NP33" s="18" t="n">
-        <v>0.6155339805825242</v>
+        <v>0.5908221797323137</v>
       </c>
       <c r="NR33" s="16" t="n">
         <v>731</v>
@@ -33378,9 +33334,7 @@
       <c r="OE33" s="18" t="n">
         <v>0.02885292047853616</v>
       </c>
-      <c r="OF33" s="18" t="n">
-        <v>0.02669247060541883</v>
-      </c>
+      <c r="OF33" s="18" t="inlineStr"/>
       <c r="OH33" s="18" t="inlineStr"/>
     </row>
     <row r="34">
@@ -35726,9 +35680,7 @@
       <c r="OE35" s="10" t="n">
         <v>-1</v>
       </c>
-      <c r="OF35" s="10" t="n">
-        <v>0</v>
-      </c>
+      <c r="OF35" s="10" t="inlineStr"/>
       <c r="OH35" s="10" t="inlineStr"/>
     </row>
     <row r="36">
@@ -36883,7 +36835,7 @@
         <v>-0.003977724741447863</v>
       </c>
       <c r="NP37" s="18" t="n">
-        <v>-0.003977724741447863</v>
+        <v>-0.037663335895465</v>
       </c>
       <c r="NR37" s="16" t="n">
         <v>1614</v>
@@ -36927,9 +36879,7 @@
       <c r="OE37" s="18" t="n">
         <v>-0.09756779424098405</v>
       </c>
-      <c r="OF37" s="18" t="n">
-        <v>0.07962506166748889</v>
-      </c>
+      <c r="OF37" s="18" t="inlineStr"/>
       <c r="OH37" s="18" t="inlineStr"/>
     </row>
     <row r="38">
@@ -38067,7 +38017,7 @@
         <v>0.2082262210796915</v>
       </c>
       <c r="NP38" s="18" t="n">
-        <v>0.2082262210796915</v>
+        <v>0.1463414634146341</v>
       </c>
       <c r="NR38" s="16" t="n">
         <v>1055</v>
@@ -38111,9 +38061,7 @@
       <c r="OE38" s="18" t="n">
         <v>-0.08400260473192966</v>
       </c>
-      <c r="OF38" s="18" t="n">
-        <v>0.07960461782237983</v>
-      </c>
+      <c r="OF38" s="18" t="inlineStr"/>
       <c r="OH38" s="18" t="inlineStr"/>
     </row>
     <row r="39">
@@ -41612,7 +41560,7 @@
         <v>0.02151096713959855</v>
       </c>
       <c r="NP42" s="18" t="n">
-        <v>0.02151096713959868</v>
+        <v>-0.01136489657275903</v>
       </c>
       <c r="NR42" s="23" t="n">
         <v>88280.77</v>
@@ -41656,9 +41604,7 @@
       <c r="OE42" s="18" t="n">
         <v>-0.04001354060617313</v>
       </c>
-      <c r="OF42" s="18" t="n">
-        <v>0.0444037027315126</v>
-      </c>
+      <c r="OF42" s="18" t="inlineStr"/>
       <c r="OH42" s="18" t="inlineStr"/>
     </row>
     <row r="43">
@@ -42796,7 +42742,7 @@
         <v>0.572265281648098</v>
       </c>
       <c r="NP43" s="18" t="n">
-        <v>0.5722652816480979</v>
+        <v>0.4959323204362706</v>
       </c>
       <c r="NR43" s="23" t="n">
         <v>16593.47</v>
@@ -42840,9 +42786,7 @@
       <c r="OE43" s="18" t="n">
         <v>0.04571460891504286</v>
       </c>
-      <c r="OF43" s="18" t="n">
-        <v>0.02986166341436359</v>
-      </c>
+      <c r="OF43" s="18" t="inlineStr"/>
       <c r="OH43" s="18" t="inlineStr"/>
     </row>
     <row r="44">
@@ -45184,9 +45128,7 @@
       <c r="OE45" s="10" t="n">
         <v>-1</v>
       </c>
-      <c r="OF45" s="10" t="n">
-        <v>0</v>
-      </c>
+      <c r="OF45" s="10" t="inlineStr"/>
       <c r="OH45" s="10" t="inlineStr"/>
     </row>
     <row r="46">
@@ -46341,7 +46283,7 @@
         <v>0.04985337243401755</v>
       </c>
       <c r="NP47" s="18" t="n">
-        <v>0.04985337243401759</v>
+        <v>0.02176239743132358</v>
       </c>
       <c r="NR47" s="23" t="n">
         <v>17595</v>
@@ -46385,9 +46327,7 @@
       <c r="OE47" s="18" t="n">
         <v>-0.101465002712968</v>
       </c>
-      <c r="OF47" s="18" t="n">
-        <v>0.07716851419361205</v>
-      </c>
+      <c r="OF47" s="18" t="inlineStr"/>
       <c r="OH47" s="18" t="inlineStr"/>
     </row>
     <row r="48">
@@ -47525,7 +47465,7 @@
         <v>0.2307692307692308</v>
       </c>
       <c r="NP48" s="18" t="n">
-        <v>0.2307692307692308</v>
+        <v>0.1586068654472563</v>
       </c>
       <c r="NR48" s="23" t="n">
         <v>12867.5</v>
@@ -47569,9 +47509,7 @@
       <c r="OE48" s="18" t="n">
         <v>-0.09677985434763536</v>
       </c>
-      <c r="OF48" s="18" t="n">
-        <v>0.07890420198985144</v>
-      </c>
+      <c r="OF48" s="18" t="inlineStr"/>
       <c r="OH48" s="18" t="inlineStr"/>
     </row>
     <row r="49">

</xml_diff>